<commit_message>
update impfzahlen corona report (+hersteller)
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-02-14.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-02-14.xlsx
@@ -14,12 +14,15 @@
     <sheet name="Vorwarnzeit" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Regionale Daten" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Internationaler Vergleich" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Geimpfte Personen" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Regional Geimpfte" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Impfstoffdosen" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="377">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -497,7 +500,7 @@
     <t xml:space="preserve">2,8 %</t>
   </si>
   <si>
-    <t xml:space="preserve">21.02.2021</t>
+    <t xml:space="preserve">03.03.2021</t>
   </si>
   <si>
     <t xml:space="preserve">Baden-Württemberg</t>
@@ -506,7 +509,7 @@
     <t xml:space="preserve">0,87</t>
   </si>
   <si>
-    <t xml:space="preserve">✓</t>
+    <t xml:space="preserve">28.02.2021</t>
   </si>
   <si>
     <t xml:space="preserve">Bayern</t>
@@ -518,7 +521,7 @@
     <t xml:space="preserve">0,82</t>
   </si>
   <si>
-    <t xml:space="preserve">20.02.2021</t>
+    <t xml:space="preserve">01.03.2021</t>
   </si>
   <si>
     <t xml:space="preserve">Berlin</t>
@@ -530,6 +533,9 @@
     <t xml:space="preserve">0,85</t>
   </si>
   <si>
+    <t xml:space="preserve">04.03.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brandenburg</t>
   </si>
   <si>
@@ -539,18 +545,12 @@
     <t xml:space="preserve">0,79</t>
   </si>
   <si>
-    <t xml:space="preserve">25.02.2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bremen</t>
   </si>
   <si>
     <t xml:space="preserve">2,5 %</t>
   </si>
   <si>
-    <t xml:space="preserve">22.02.2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hamburg</t>
   </si>
   <si>
@@ -560,21 +560,21 @@
     <t xml:space="preserve">0,90</t>
   </si>
   <si>
-    <t xml:space="preserve">03.03.2021</t>
+    <t xml:space="preserve">20.03.2021</t>
   </si>
   <si>
     <t xml:space="preserve">Hessen</t>
   </si>
   <si>
-    <t xml:space="preserve">19.02.2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mecklenburg-Vorpommern</t>
   </si>
   <si>
     <t xml:space="preserve">1,4 %</t>
   </si>
   <si>
+    <t xml:space="preserve">08.03.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Niedersachsen</t>
   </si>
   <si>
@@ -584,7 +584,7 @@
     <t xml:space="preserve">0,91</t>
   </si>
   <si>
-    <t xml:space="preserve">04.03.2021</t>
+    <t xml:space="preserve">22.03.2021</t>
   </si>
   <si>
     <t xml:space="preserve">Nordrhein-Westfalen</t>
@@ -596,7 +596,7 @@
     <t xml:space="preserve">2,4 %</t>
   </si>
   <si>
-    <t xml:space="preserve">17.02.2021</t>
+    <t xml:space="preserve">26.02.2021</t>
   </si>
   <si>
     <t xml:space="preserve">Saarland</t>
@@ -605,7 +605,7 @@
     <t xml:space="preserve">0,81</t>
   </si>
   <si>
-    <t xml:space="preserve">24.02.2021</t>
+    <t xml:space="preserve">05.03.2021</t>
   </si>
   <si>
     <t xml:space="preserve">Sachsen</t>
@@ -617,9 +617,6 @@
     <t xml:space="preserve">0,76</t>
   </si>
   <si>
-    <t xml:space="preserve">23.02.2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sachsen-Anhalt</t>
   </si>
   <si>
@@ -632,15 +629,15 @@
     <t xml:space="preserve">Schleswig-Holstein</t>
   </si>
   <si>
+    <t xml:space="preserve">12.03.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thüringen</t>
   </si>
   <si>
     <t xml:space="preserve">3,3 %</t>
   </si>
   <si>
-    <t xml:space="preserve">27.02.2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fälle gesamt</t>
   </si>
   <si>
@@ -765,6 +762,405 @@
   </si>
   <si>
     <t xml:space="preserve"> 4,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geimpfte Personen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand 17.2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamt-Bevölkerung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2896064 ( 3,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit nur 1 Impfung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1370121 ( 1,6 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit 2 Impfungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1525943 ( 1,8 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pflegeheimbewohnende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">724275 (91,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">263545 (33,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">460730 (58,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Über-80-Jährige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1134114 (20,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">596589 (10,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">537525 ( 9,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal in ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1315447 (36,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">578760 (16,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">736687 (20,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamt nur 1x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gesamt 2x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHB nur 1x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHB 2x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter nur 1x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter 2x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impfquote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-Tage-Inzidenz 80+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impfstoffdosen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dieseWoche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verabreichte Impfstoffdosen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4422007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstimpfungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2896064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zweitimpfungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1525943</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nach Herstellern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biontech/Pfizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4234503 ( 95,8 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2723359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1511144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99971 (  2,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AstraZeneca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87533 (  2,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87533</t>
   </si>
 </sst>
 </file>
@@ -1186,6 +1582,724 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2" t="n">
+        <v>58</v>
+      </c>
+      <c r="J2" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H3" t="s">
+        <v>283</v>
+      </c>
+      <c r="I3" t="n">
+        <v>43</v>
+      </c>
+      <c r="J3" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F4" t="s">
+        <v>287</v>
+      </c>
+      <c r="G4" t="s">
+        <v>288</v>
+      </c>
+      <c r="H4" t="s">
+        <v>289</v>
+      </c>
+      <c r="I4" t="n">
+        <v>56</v>
+      </c>
+      <c r="J4" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D5" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G5" t="s">
+        <v>294</v>
+      </c>
+      <c r="H5" t="s">
+        <v>289</v>
+      </c>
+      <c r="I5" t="n">
+        <v>50</v>
+      </c>
+      <c r="J5" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E6" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G6" t="s">
+        <v>300</v>
+      </c>
+      <c r="H6" t="s">
+        <v>283</v>
+      </c>
+      <c r="I6" t="n">
+        <v>72</v>
+      </c>
+      <c r="J6" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D7" t="s">
+        <v>303</v>
+      </c>
+      <c r="E7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F7" t="s">
+        <v>287</v>
+      </c>
+      <c r="G7" t="s">
+        <v>227</v>
+      </c>
+      <c r="H7" t="s">
+        <v>289</v>
+      </c>
+      <c r="I7" t="n">
+        <v>64</v>
+      </c>
+      <c r="J7" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E8" t="s">
+        <v>306</v>
+      </c>
+      <c r="F8" t="s">
+        <v>307</v>
+      </c>
+      <c r="G8" t="s">
+        <v>308</v>
+      </c>
+      <c r="H8" t="s">
+        <v>289</v>
+      </c>
+      <c r="I8" t="n">
+        <v>58</v>
+      </c>
+      <c r="J8" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" t="s">
+        <v>310</v>
+      </c>
+      <c r="F9" t="s">
+        <v>311</v>
+      </c>
+      <c r="G9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H9" t="s">
+        <v>312</v>
+      </c>
+      <c r="I9" t="n">
+        <v>55</v>
+      </c>
+      <c r="J9" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D10" t="s">
+        <v>313</v>
+      </c>
+      <c r="E10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F10" t="s">
+        <v>315</v>
+      </c>
+      <c r="G10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H10" t="s">
+        <v>317</v>
+      </c>
+      <c r="I10" t="n">
+        <v>64</v>
+      </c>
+      <c r="J10" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11" t="s">
+        <v>272</v>
+      </c>
+      <c r="D11" t="s">
+        <v>319</v>
+      </c>
+      <c r="E11" t="s">
+        <v>320</v>
+      </c>
+      <c r="F11" t="s">
+        <v>315</v>
+      </c>
+      <c r="G11" t="s">
+        <v>321</v>
+      </c>
+      <c r="H11" t="s">
+        <v>322</v>
+      </c>
+      <c r="I11" t="n">
+        <v>66</v>
+      </c>
+      <c r="J11" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D12" t="s">
+        <v>323</v>
+      </c>
+      <c r="E12" t="s">
+        <v>324</v>
+      </c>
+      <c r="F12" t="s">
+        <v>325</v>
+      </c>
+      <c r="G12" t="s">
+        <v>326</v>
+      </c>
+      <c r="H12" t="s">
+        <v>277</v>
+      </c>
+      <c r="I12" t="n">
+        <v>56</v>
+      </c>
+      <c r="J12" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" t="s">
+        <v>328</v>
+      </c>
+      <c r="D13" t="s">
+        <v>329</v>
+      </c>
+      <c r="E13" t="s">
+        <v>330</v>
+      </c>
+      <c r="F13" t="s">
+        <v>331</v>
+      </c>
+      <c r="G13" t="s">
+        <v>332</v>
+      </c>
+      <c r="H13" t="s">
+        <v>289</v>
+      </c>
+      <c r="I13" t="n">
+        <v>45</v>
+      </c>
+      <c r="J13" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C14" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" t="s">
+        <v>334</v>
+      </c>
+      <c r="E14" t="s">
+        <v>335</v>
+      </c>
+      <c r="F14" t="s">
+        <v>336</v>
+      </c>
+      <c r="G14" t="s">
+        <v>337</v>
+      </c>
+      <c r="H14" t="s">
+        <v>338</v>
+      </c>
+      <c r="I14" t="n">
+        <v>62</v>
+      </c>
+      <c r="J14" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" t="s">
+        <v>278</v>
+      </c>
+      <c r="C15" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" t="s">
+        <v>339</v>
+      </c>
+      <c r="E15" t="s">
+        <v>340</v>
+      </c>
+      <c r="F15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G15" t="s">
+        <v>342</v>
+      </c>
+      <c r="H15" t="s">
+        <v>283</v>
+      </c>
+      <c r="I15" t="n">
+        <v>65</v>
+      </c>
+      <c r="J15" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" t="s">
+        <v>343</v>
+      </c>
+      <c r="C16" t="s">
+        <v>333</v>
+      </c>
+      <c r="D16" t="s">
+        <v>344</v>
+      </c>
+      <c r="E16" t="s">
+        <v>345</v>
+      </c>
+      <c r="F16" t="s">
+        <v>346</v>
+      </c>
+      <c r="G16" t="s">
+        <v>347</v>
+      </c>
+      <c r="H16" t="s">
+        <v>312</v>
+      </c>
+      <c r="I16" t="n">
+        <v>85</v>
+      </c>
+      <c r="J16" t="n">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" t="s">
+        <v>348</v>
+      </c>
+      <c r="E17" t="s">
+        <v>349</v>
+      </c>
+      <c r="F17" t="s">
+        <v>350</v>
+      </c>
+      <c r="G17" t="s">
+        <v>351</v>
+      </c>
+      <c r="H17" t="s">
+        <v>289</v>
+      </c>
+      <c r="I17" t="n">
+        <v>56</v>
+      </c>
+      <c r="J17" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" t="s">
+        <v>333</v>
+      </c>
+      <c r="D18" t="s">
+        <v>353</v>
+      </c>
+      <c r="E18" t="s">
+        <v>354</v>
+      </c>
+      <c r="F18" t="s">
+        <v>355</v>
+      </c>
+      <c r="G18" t="s">
+        <v>356</v>
+      </c>
+      <c r="H18" t="s">
+        <v>317</v>
+      </c>
+      <c r="I18" t="n">
+        <v>112</v>
+      </c>
+      <c r="J18" t="n">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>365</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>370</v>
+      </c>
+      <c r="B10" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>363</v>
+      </c>
+      <c r="B12" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>374</v>
+      </c>
+      <c r="B13" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>361</v>
+      </c>
+      <c r="B14" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>363</v>
+      </c>
+      <c r="B15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
@@ -1932,21 +3046,21 @@
         <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C6" t="n">
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E6" t="n">
         <v>78</v>
@@ -1955,7 +3069,7 @@
         <v>76</v>
       </c>
       <c r="G6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7">
@@ -1978,21 +3092,21 @@
         <v>63</v>
       </c>
       <c r="G7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
         <v>174</v>
-      </c>
-      <c r="B8" t="s">
-        <v>175</v>
       </c>
       <c r="C8" t="n">
         <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E8" t="n">
         <v>64</v>
@@ -2001,15 +3115,15 @@
         <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C9" t="n">
         <v>58</v>
@@ -2024,15 +3138,15 @@
         <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" t="n">
         <v>53</v>
@@ -2047,21 +3161,21 @@
         <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" t="s">
         <v>182</v>
-      </c>
-      <c r="B11" t="s">
-        <v>183</v>
       </c>
       <c r="C11" t="n">
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E11" t="n">
         <v>58</v>
@@ -2070,12 +3184,12 @@
         <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B12" t="s">
         <v>155</v>
@@ -2098,10 +3212,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" t="s">
         <v>187</v>
-      </c>
-      <c r="B13" t="s">
-        <v>188</v>
       </c>
       <c r="C13" t="n">
         <v>62</v>
@@ -2116,12 +3230,12 @@
         <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
         <v>155</v>
@@ -2130,7 +3244,7 @@
         <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E14" t="n">
         <v>67</v>
@@ -2139,21 +3253,21 @@
         <v>71</v>
       </c>
       <c r="G14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" t="s">
         <v>193</v>
-      </c>
-      <c r="B15" t="s">
-        <v>194</v>
       </c>
       <c r="C15" t="n">
         <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E15" t="n">
         <v>77</v>
@@ -2162,21 +3276,21 @@
         <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C16" t="n">
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E16" t="n">
         <v>89</v>
@@ -2185,21 +3299,21 @@
         <v>82</v>
       </c>
       <c r="G16" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C17" t="n">
         <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17" t="n">
         <v>54</v>
@@ -2208,21 +3322,21 @@
         <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" t="s">
         <v>201</v>
-      </c>
-      <c r="B18" t="s">
-        <v>202</v>
       </c>
       <c r="C18" t="n">
         <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E18" t="n">
         <v>100</v>
@@ -2231,7 +3345,7 @@
         <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2250,48 +3364,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>204</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>205</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>206</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>207</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>208</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>209</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>210</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>211</v>
-      </c>
-      <c r="I1" t="s">
-        <v>212</v>
-      </c>
-      <c r="J1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C2" t="n">
         <v>1088009</v>
       </c>
       <c r="D2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E2" t="s">
         <v>165</v>
@@ -2300,62 +3414,62 @@
         <v>93577</v>
       </c>
       <c r="G2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H2" t="n">
         <v>966</v>
       </c>
       <c r="I2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" t="s">
         <v>217</v>
-      </c>
-      <c r="B3" t="s">
-        <v>219</v>
       </c>
       <c r="C3" t="n">
         <v>785756</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F3" t="n">
         <v>117387</v>
       </c>
       <c r="G3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H3" t="n">
         <v>670</v>
       </c>
       <c r="I3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" t="s">
         <v>221</v>
-      </c>
-      <c r="B4" t="s">
-        <v>223</v>
       </c>
       <c r="C4" t="n">
         <v>3056035</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E4" t="s">
         <v>155</v>
@@ -2364,62 +3478,62 @@
         <v>65107</v>
       </c>
       <c r="G4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H4" t="n">
         <v>638</v>
       </c>
       <c r="I4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C5" t="n">
         <v>1043541</v>
       </c>
       <c r="D5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F5" t="n">
         <v>40807</v>
       </c>
       <c r="G5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H5" t="n">
         <v>328</v>
       </c>
       <c r="I5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C6" t="n">
         <v>4049920</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E6" t="s">
         <v>172</v>
@@ -2428,149 +3542,149 @@
         <v>19366</v>
       </c>
       <c r="G6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H6" t="n">
         <v>325</v>
       </c>
       <c r="I6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" t="s">
         <v>232</v>
-      </c>
-      <c r="B7" t="s">
-        <v>234</v>
       </c>
       <c r="C7" t="n">
         <v>3467884</v>
       </c>
       <c r="D7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F7" t="n">
         <v>80961</v>
       </c>
       <c r="G7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H7" t="n">
         <v>301</v>
       </c>
       <c r="I7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C8" t="n">
         <v>2721879</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F8" t="n">
         <v>64747</v>
       </c>
       <c r="G8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H8" t="n">
         <v>279</v>
       </c>
       <c r="I8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C9" t="n">
         <v>1588955</v>
       </c>
       <c r="D9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F9" t="n">
         <v>15321</v>
       </c>
       <c r="G9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H9" t="n">
         <v>199</v>
       </c>
       <c r="I9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C10" t="n">
         <v>761963</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F10" t="n">
         <v>18143</v>
       </c>
       <c r="G10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H10" t="n">
         <v>172</v>
       </c>
       <c r="I10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s">
         <v>155</v>
@@ -2579,25 +3693,167 @@
         <v>2341744</v>
       </c>
       <c r="D11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F11" t="n">
         <v>14936</v>
       </c>
       <c r="G11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H11" t="n">
         <v>139</v>
       </c>
       <c r="I11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" t="s">
         <v>245</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>